<commit_message>
Adding Smart Folder deprecation check.
</commit_message>
<xml_diff>
--- a/ota-bom/resources/findings.xlsx
+++ b/ota-bom/resources/findings.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Work\OfferingManagement\4Projects\OTA\odm-transformation-advisor\ota-bom\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\4Work\GarageSolutionEngineering\Workstreams\OTA\odm-transformation-advisor\ota-bom\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641E197E-01C8-4625-8F92-1AA6DEEF8BC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15324" windowHeight="2904" tabRatio="314" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="314" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="findings" sheetId="1" r:id="rId1"/>
     <sheet name="markers" sheetId="2" r:id="rId2"/>
     <sheet name="parameters" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="169">
   <si>
     <t>CLASSIC_PROJECT</t>
   </si>
@@ -480,12 +489,66 @@
   <si>
     <t>N/A for SaaS</t>
   </si>
+  <si>
+    <t>Smart Folder defined</t>
+  </si>
+  <si>
+    <t>Smart Folders</t>
+  </si>
+  <si>
+    <t>return "SMART_FOLDER";</t>
+  </si>
+  <si>
+    <t>UPDATE_STATE</t>
+  </si>
+  <si>
+    <t>Member using update object state</t>
+  </si>
+  <si>
+    <t>Member Using Update State</t>
+  </si>
+  <si>
+    <t>return "UPDATE_STATE";</t>
+  </si>
+  <si>
+    <t>SMART_FOLDER</t>
+  </si>
+  <si>
+    <t>PERMISSIONS</t>
+  </si>
+  <si>
+    <t>Group using fine-grained permissions</t>
+  </si>
+  <si>
+    <t>Some rule projects are using Smart Folders (for example, &lt;em&gt;%2$s&lt;/em&gt; in project &lt;em&gt;%1$s&lt;/em&gt;). Decision Trees have been deprecated since ODM version 8.10.0. &lt;br&gt;&lt;br&gt;&lt;b&gt;%3$s occurence%4$s found&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Some BOM members are using the "Update object state" option. One example is &lt;em&gt;%2$s&lt;/em&gt; in project &lt;em&gt;%1$s&lt;/em&gt;. This option is only useful when performing inference with the RetePlus algorithm. Make sure the use of this option is intentional in the context of your rules. &lt;br&gt;&lt;br&gt;&lt;b&gt;%3$s occurence%4$s found&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Fine Grained Permissions</t>
+  </si>
+  <si>
+    <t>return "PERMISSIONS";</t>
+  </si>
+  <si>
+    <t>maxB2XCharSize</t>
+  </si>
+  <si>
+    <t>Max B2X Char Size</t>
+  </si>
+  <si>
+    <t>return "maxB2XCharSize";</t>
+  </si>
+  <si>
+    <t>Some user groups are associated with fine-grained permissions on repository artifacts (for instance, the custom group &lt;em&gt;%1$s&lt;/em&gt; defines &lt;em&gt;%2$s&lt;/em&gt; such permissions). These fine-grained permissions are deprecated in ODM 8.10.0. The migration path is to rely on the assigned authors, testers and approvers in the release and activities from the Governance Framework. &lt;br&gt;&lt;br&gt;&lt;b&gt;%3$s occurence%4$s found&lt;/b&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,6 +560,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -522,7 +598,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -545,11 +621,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -573,10 +725,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,27 +1046,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -898,11 +1088,11 @@
       <c r="G1" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -921,12 +1111,12 @@
       <c r="F2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -945,12 +1135,12 @@
       <c r="F3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -969,14 +1159,14 @@
       <c r="F4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="12" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -995,12 +1185,12 @@
       <c r="F5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H5" s="9"/>
+      <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1019,12 +1209,12 @@
       <c r="F6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="9"/>
+      <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
@@ -1043,12 +1233,12 @@
       <c r="F7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>38</v>
       </c>
@@ -1067,12 +1257,12 @@
       <c r="F8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>42</v>
       </c>
@@ -1091,12 +1281,12 @@
       <c r="F9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>45</v>
       </c>
@@ -1115,12 +1305,12 @@
       <c r="F10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>52</v>
       </c>
@@ -1139,12 +1329,12 @@
       <c r="F11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>70</v>
       </c>
@@ -1163,12 +1353,12 @@
       <c r="F12" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>74</v>
       </c>
@@ -1187,12 +1377,12 @@
       <c r="F13" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>78</v>
       </c>
@@ -1211,12 +1401,12 @@
       <c r="F14" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>84</v>
       </c>
@@ -1235,12 +1425,12 @@
       <c r="F15" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>90</v>
       </c>
@@ -1259,12 +1449,12 @@
       <c r="F16" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>95</v>
       </c>
@@ -1283,12 +1473,12 @@
       <c r="F17" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="9"/>
+      <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>99</v>
       </c>
@@ -1307,12 +1497,12 @@
       <c r="F18" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>106</v>
       </c>
@@ -1331,12 +1521,12 @@
       <c r="F19" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>111</v>
       </c>
@@ -1355,12 +1545,12 @@
       <c r="F20" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>114</v>
       </c>
@@ -1379,12 +1569,12 @@
       <c r="F21" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>123</v>
       </c>
@@ -1403,12 +1593,12 @@
       <c r="F22" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>126</v>
       </c>
@@ -1427,12 +1617,12 @@
       <c r="F23" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>137</v>
       </c>
@@ -1451,60 +1641,133 @@
       <c r="F24" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H24" s="9"/>
+      <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="12" t="s">
         <v>143</v>
       </c>
+    </row>
+    <row r="26" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16384" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -17900,54 +18163,54 @@
       <c r="XFC1" s="3"/>
       <c r="XFD1" s="3"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>3</v>
       </c>
     </row>
@@ -17957,20 +18220,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -17981,15 +18245,26 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="23" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>